<commit_message>
added excel import test
</commit_message>
<xml_diff>
--- a/ganttproject-builder/dist-bin/Livro1.xlsx
+++ b/ganttproject-builder/dist-bin/Livro1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dany5\Desktop\ganttproject\ganttproject-builder\dist-bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9843CA7C-5569-42D5-9255-2778EB2B2E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8329FB-3913-40A9-A6FD-B096AA729BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2892" yWindow="2820" windowWidth="17280" windowHeight="9420" xr2:uid="{57E7BB9E-FE34-4A12-914F-67811222C44F}"/>
+    <workbookView xWindow="3240" yWindow="2820" windowWidth="17280" windowHeight="9420" xr2:uid="{57E7BB9E-FE34-4A12-914F-67811222C44F}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Daniel</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Guilherme</t>
   </si>
   <si>
-    <t>Actor</t>
-  </si>
-  <si>
     <t>Miguel</t>
   </si>
   <si>
@@ -71,13 +68,13 @@
     <t>gj.abrantes@campus.fct.unl.pt</t>
   </si>
   <si>
-    <t>Yolo</t>
-  </si>
-  <si>
-    <t>yolo.pepino@campus.fct.unl.pt</t>
-  </si>
-  <si>
-    <t>pesoMorto</t>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>f.silveira@campus.fct.unl.pt</t>
   </si>
 </sst>
 </file>
@@ -443,7 +440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BAA5D3B-3381-4A82-9FCA-20553AF133DD}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -492,24 +491,24 @@
         <v>912323234</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>934545469</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -529,10 +528,10 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>